<commit_message>
Continue Sign in ...
</commit_message>
<xml_diff>
--- a/FileString/FSANDROID/DataSet/DataSignIn.xlsx
+++ b/FileString/FSANDROID/DataSet/DataSignIn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="9360" tabRatio="891" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="9360" tabRatio="891" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1000" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>sta281@yopmail.com</t>
   </si>
@@ -92,6 +92,30 @@
   </si>
   <si>
     <t>staandroidsecondunverify@yopmail.com</t>
+  </si>
+  <si>
+    <t>${v_result}=</t>
+  </si>
+  <si>
+    <t>Run Keyword And Ignore Error</t>
+  </si>
+  <si>
+    <t>AppiumLibrary.Click Element</t>
+  </si>
+  <si>
+    <t>${Home_Back}</t>
+  </si>
+  <si>
+    <t>Run Keyword If</t>
+  </si>
+  <si>
+    <t>'${v_result[0]}'=='FAIL'</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Can not close What's New</t>
   </si>
 </sst>
 </file>
@@ -697,7 +721,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,43 +749,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="sta281@yopmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1234</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="sta281@yopmail.com"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -825,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>